<commit_message>
Project plan fix for infrastructure and acceptance
</commit_message>
<xml_diff>
--- a/Project Status.xlsx
+++ b/Project Status.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ronaldo\Dropbox\UTD\Courses\Project Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ronaldo\Documents\GitHub\comitbites-documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -288,23 +288,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -340,23 +323,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -512,7 +478,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -555,7 +521,7 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="2"/>
       <c r="C4" s="1" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Project Status updated to match deliverables 3
</commit_message>
<xml_diff>
--- a/Project Status.xlsx
+++ b/Project Status.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
   <si>
     <t>Feasibility</t>
   </si>
@@ -116,9 +116,6 @@
     <t>Demo - Place Order</t>
   </si>
   <si>
-    <t>keerthi</t>
-  </si>
-  <si>
     <t>ram</t>
   </si>
   <si>
@@ -131,13 +128,13 @@
     <t>section 6, twinkle</t>
   </si>
   <si>
-    <t>2pm</t>
-  </si>
-  <si>
-    <t>after OC</t>
-  </si>
-  <si>
-    <t>after</t>
+    <t>redo</t>
+  </si>
+  <si>
+    <t>pause</t>
+  </si>
+  <si>
+    <t>needs review</t>
   </si>
 </sst>
 </file>
@@ -185,11 +182,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -505,7 +503,7 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
@@ -526,7 +524,7 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
@@ -560,12 +558,12 @@
       <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="2"/>
       <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
@@ -577,19 +575,19 @@
         <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="2"/>
       <c r="C10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
@@ -601,7 +599,7 @@
         <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
@@ -617,29 +615,26 @@
       <c r="A13" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="3"/>
+      <c r="B13" s="2"/>
       <c r="C13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D13" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" t="s">
-        <v>37</v>
+      <c r="B14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="1" t="s">
@@ -648,7 +643,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="1" t="s">
@@ -657,37 +652,37 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="1" t="s">
-        <v>14</v>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D21" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="1" t="s">
@@ -696,7 +691,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="1" t="s">
@@ -705,7 +700,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="1" t="s">
@@ -714,25 +709,25 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="1" t="s">
-        <v>20</v>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="1" t="s">
@@ -741,7 +736,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="1" t="s">
@@ -750,7 +745,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="1" t="s">
@@ -759,19 +754,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
-        <v>19</v>
-      </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="1" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated documents (deliverables 4)
</commit_message>
<xml_diff>
--- a/Project Status.xlsx
+++ b/Project Status.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="53">
   <si>
     <t>Feasibility</t>
   </si>
@@ -135,6 +135,54 @@
   </si>
   <si>
     <t>needs review</t>
+  </si>
+  <si>
+    <t>ronaldo</t>
+  </si>
+  <si>
+    <t>keerthi</t>
+  </si>
+  <si>
+    <t>twinkle</t>
+  </si>
+  <si>
+    <t>main screen</t>
+  </si>
+  <si>
+    <t>food joint selection</t>
+  </si>
+  <si>
+    <t>menu</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>browse</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>make payment</t>
+  </si>
+  <si>
+    <t>e-ticket</t>
+  </si>
+  <si>
+    <t>cancel order</t>
+  </si>
+  <si>
+    <t>error msg</t>
+  </si>
+  <si>
+    <t>log in</t>
+  </si>
+  <si>
+    <t>Cloud environment</t>
   </si>
 </sst>
 </file>
@@ -286,6 +334,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -321,6 +386,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -473,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -484,9 +566,14 @@
     <col min="1" max="1" width="23.265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.06640625" style="1"/>
     <col min="4" max="4" width="27.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.9296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>7</v>
       </c>
@@ -494,7 +581,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -506,7 +593,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -515,7 +602,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -527,7 +614,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -536,7 +623,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -545,7 +632,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -554,7 +641,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -566,7 +653,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -578,7 +665,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -590,7 +677,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -602,7 +689,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -610,8 +697,14 @@
       <c r="C12" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="G12" t="s">
+        <v>50</v>
+      </c>
+      <c r="H12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -619,26 +712,65 @@
       <c r="C13" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B14" s="4"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="3"/>
+      <c r="B15" s="2"/>
       <c r="C15" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" t="s">
+        <v>42</v>
+      </c>
+      <c r="H15" t="s">
+        <v>45</v>
+      </c>
+      <c r="I15" t="s">
+        <v>47</v>
+      </c>
+      <c r="J15" t="s">
+        <v>48</v>
+      </c>
+      <c r="K15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="3"/>
+      <c r="B16" s="2"/>
       <c r="C16" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="D16" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
@@ -649,12 +781,15 @@
       <c r="C17" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="D17" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="3"/>
+      <c r="B18" s="2"/>
       <c r="C18" s="1" t="s">
         <v>14</v>
       </c>
@@ -663,7 +798,7 @@
       <c r="A20" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="3"/>
+      <c r="B20" s="2"/>
       <c r="C20" s="1" t="s">
         <v>20</v>
       </c>
@@ -675,7 +810,7 @@
       <c r="A21" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="3"/>
+      <c r="B21" s="2"/>
       <c r="C21" s="1" t="s">
         <v>20</v>
       </c>
@@ -684,7 +819,7 @@
       <c r="A22" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="3"/>
+      <c r="B22" s="2"/>
       <c r="C22" s="1" t="s">
         <v>20</v>
       </c>
@@ -697,12 +832,15 @@
       <c r="C23" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="D23" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="3"/>
+      <c r="B24" s="2"/>
       <c r="C24" s="1" t="s">
         <v>20</v>
       </c>
@@ -716,18 +854,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="1" t="s">
-        <v>25</v>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="1" t="s">
@@ -736,7 +874,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="1" t="s">
@@ -745,7 +883,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="1" t="s">
@@ -754,14 +892,24 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="1" t="s">
         <v>25</v>
       </c>
     </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added pdf versions for delivery
</commit_message>
<xml_diff>
--- a/Project Status.xlsx
+++ b/Project Status.xlsx
@@ -557,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Moved cloud files to the right folder
</commit_message>
<xml_diff>
--- a/Project Status.xlsx
+++ b/Project Status.xlsx
@@ -189,10 +189,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -230,12 +237,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -828,7 +836,7 @@
       <c r="A23" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="3"/>
+      <c r="B23" s="5"/>
       <c r="C23" s="1" t="s">
         <v>20</v>
       </c>
@@ -849,7 +857,7 @@
       <c r="A25" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="3"/>
+      <c r="B25" s="2"/>
       <c r="C25" s="1" t="s">
         <v>20</v>
       </c>
@@ -858,7 +866,7 @@
       <c r="A26" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="3"/>
+      <c r="B26" s="2"/>
       <c r="C26" s="1" t="s">
         <v>20</v>
       </c>

</xml_diff>